<commit_message>
Updated pspec:spec:parsetitle for NAI.  Added tagged hbin inputs for HIY16/ATM18
</commit_message>
<xml_diff>
--- a/linelist/LineLists_Map.xlsx
+++ b/linelist/LineLists_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesw/FDP/sfit/400/github/sfit-core-code/linelist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBA9608-D3F4-FC49-AA44-DFDC9B9B6C0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4C0EFE-046F-054B-A87B-97F56BBC7B98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13440" yWindow="580" windowWidth="26860" windowHeight="28020" activeTab="1" xr2:uid="{25443D72-56D3-084B-8A33-DEFF1CD3507B}"/>
   </bookViews>
@@ -782,6 +782,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,9 +793,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3183,8 +3183,8 @@
   <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
+      <pane ySplit="12" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3228,28 +3228,28 @@
     </row>
     <row r="11" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="18" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="13" t="s">
         <v>181</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="N11" s="19"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
       <c r="N12" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="18" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5064,7 +5064,9 @@
       <c r="F77" s="3">
         <v>1</v>
       </c>
-      <c r="G77" s="16"/>
+      <c r="G77" s="16">
+        <v>39</v>
+      </c>
       <c r="H77" s="3" t="s">
         <v>129</v>
       </c>
@@ -5157,7 +5159,9 @@
       <c r="F82" s="3">
         <v>1</v>
       </c>
-      <c r="G82" s="16"/>
+      <c r="G82" s="16">
+        <v>41</v>
+      </c>
       <c r="H82" s="3" t="s">
         <v>138</v>
       </c>

</xml_diff>